<commit_message>
apparence de l'applciation terminé
</commit_message>
<xml_diff>
--- a/B65_S1_Conception_Afsaneh_Sheikhmiri/B65_S1_Planification_AfsanehSheikhmiri.xlsx
+++ b/B65_S1_Conception_Afsaneh_Sheikhmiri/B65_S1_Planification_AfsanehSheikhmiri.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/afsanehsheikhmiri/Documents/Afsaneh/Graduation_project/B65_S1_Conception_Afsaneh_Sheikhmiri/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/afsanehsheikhmiri/Documents/Afsaneh/git_graduation_project/projet_synthese_HIV2020/B65_S1_Conception_Afsaneh_Sheikhmiri/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" tabRatio="494" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" tabRatio="494"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1 - Planification" sheetId="1" r:id="rId1"/>
@@ -3605,8 +3605,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="-378988848"/>
-        <c:axId val="-378987488"/>
+        <c:axId val="1835328800"/>
+        <c:axId val="1835330848"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -3656,13 +3656,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>7.0</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.0</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18.0</c:v>
+                  <c:v>17.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3679,11 +3679,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-378988848"/>
-        <c:axId val="-378987488"/>
+        <c:axId val="1835328800"/>
+        <c:axId val="1835330848"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-378988848"/>
+        <c:axId val="1835328800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3726,7 +3726,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-378987488"/>
+        <c:crossAx val="1835330848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3734,7 +3734,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-378987488"/>
+        <c:axId val="1835330848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3785,7 +3785,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-378988848"/>
+        <c:crossAx val="1835328800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4065,7 +4065,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>15.0</c:v>
+                  <c:v>15.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.0</c:v>
@@ -4087,11 +4087,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-15"/>
-        <c:axId val="-335086000"/>
-        <c:axId val="-335092144"/>
+        <c:axId val="1833418544"/>
+        <c:axId val="1833421296"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-335086000"/>
+        <c:axId val="1833418544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4134,7 +4134,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-335092144"/>
+        <c:crossAx val="1833421296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4142,7 +4142,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-335092144"/>
+        <c:axId val="1833421296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4193,7 +4193,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-335086000"/>
+        <c:crossAx val="1833418544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7759,7 +7759,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AJ90"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
@@ -10610,8 +10610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:W56"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10668,7 +10668,7 @@
       <c r="F5" s="35"/>
       <c r="G5" s="64" t="str">
         <f>IF(K44=0,CONCATENATE("Ce sprint totalise ", U14, " de travail réalisé. ",U15),CONCATENATE("Attention, il reste ",K45," à remplir!"))</f>
-        <v>Attention, il reste 10 champs à remplir!</v>
+        <v>Attention, il reste 8 champs à remplir!</v>
       </c>
     </row>
     <row r="6" spans="2:23" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -10732,15 +10732,15 @@
       </c>
       <c r="Q8" s="61">
         <f t="array" ref="Q8">SUM(($D$8:$D$42=$P8)*$E$8:$E$42)</f>
-        <v>0.62499999999999922</v>
+        <v>0.64583333333333248</v>
       </c>
       <c r="R8" s="62">
         <f>Q8*24*60</f>
-        <v>899.99999999999898</v>
+        <v>929.99999999999875</v>
       </c>
       <c r="T8" s="9">
         <f>SUM(E8:E42)</f>
-        <v>0.62499999999999922</v>
+        <v>0.64583333333333248</v>
       </c>
     </row>
     <row r="9" spans="2:23" x14ac:dyDescent="0.2">
@@ -10788,7 +10788,7 @@
       </c>
       <c r="T9" s="10">
         <f>T8</f>
-        <v>0.62499999999999922</v>
+        <v>0.64583333333333248</v>
       </c>
     </row>
     <row r="10" spans="2:23" x14ac:dyDescent="0.2">
@@ -10880,7 +10880,7 @@
       <c r="P11" s="8"/>
       <c r="T11" s="4">
         <f>MINUTE(T8)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="2:23" x14ac:dyDescent="0.2">
@@ -10941,16 +10941,20 @@
         <f>IF(LEN('Sprint 1 - Planification'!H13)&lt;&gt;0,'Sprint 1 - Planification'!H13,"")</f>
         <v>Sprint 1</v>
       </c>
-      <c r="E13" s="112"/>
-      <c r="F13" s="113"/>
+      <c r="E13" s="112">
+        <v>2.0833333333333301E-2</v>
+      </c>
+      <c r="F13" s="113">
+        <v>1</v>
+      </c>
       <c r="G13" s="114"/>
       <c r="K13" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L13" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13" s="3" t="b">
         <f t="shared" si="2"/>
@@ -10962,11 +10966,11 @@
       </c>
       <c r="T13" s="4">
         <f>T11</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="U13" s="4" t="str">
         <f>T13 &amp; " " &amp; S13 &amp; IF(T13 &gt; 1, "s", "")</f>
-        <v>0 minute</v>
+        <v>30 minutes</v>
       </c>
     </row>
     <row r="14" spans="2:23" x14ac:dyDescent="0.2">
@@ -11000,11 +11004,11 @@
       <c r="P14" s="8"/>
       <c r="U14" s="4" t="str">
         <f>IF(T12&gt;0,IF(T13&gt;0,U12&amp;" et "&amp;U13,U12),U13)</f>
-        <v>15 heures</v>
+        <v>15 heures et 30 minutes</v>
       </c>
       <c r="W14" s="4" t="str">
         <f>T12&amp;"h"&amp;TEXT(T13,"00")</f>
-        <v>15h00</v>
+        <v>15h30</v>
       </c>
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.2">
@@ -11038,11 +11042,11 @@
       <c r="P15" s="8"/>
       <c r="T15" s="4">
         <f t="array" ref="T15">SUM(($D$8:$D$42="Sprint 1")*($F$8:$F$42&lt;1))</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U15" s="4" t="str">
         <f>IF(T15=0,"",IF(T15=1,"Une tâche est en retard!",CONCATENATE(T15," tâches sont en retard!")))</f>
-        <v>7 tâches sont en retard!</v>
+        <v>6 tâches sont en retard!</v>
       </c>
     </row>
     <row r="16" spans="2:23" x14ac:dyDescent="0.2">
@@ -11858,11 +11862,11 @@
     <row r="43" spans="2:16" x14ac:dyDescent="0.2">
       <c r="K43" s="3">
         <f>COUNTIF(K8:K42,TRUE)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L43" s="3">
         <f t="shared" ref="L43:M43" si="4">COUNTIF(L8:L42,TRUE)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M43" s="3">
         <f t="shared" si="4"/>
@@ -11873,14 +11877,14 @@
     <row r="44" spans="2:16" x14ac:dyDescent="0.2">
       <c r="K44" s="3">
         <f>SUM(K43:M43)</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="P44" s="8"/>
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.2">
       <c r="K45" s="3" t="str">
         <f>IF(K44=0, "aucun champ", IF(K44=1, "1 champ", K44 &amp; " champs"))</f>
-        <v>10 champs</v>
+        <v>8 champs</v>
       </c>
       <c r="P45" s="8"/>
     </row>
@@ -12108,7 +12112,7 @@
       <c r="H5" s="35"/>
       <c r="I5" s="64" t="str">
         <f>IF(M45=0,CONCATENATE("Ce sprint totalise ", W15, " de travail réalisé. ",W16),CONCATENATE("Attention, il reste ",M46," à remplir!"))</f>
-        <v>Attention, il reste 24 champs à remplir!</v>
+        <v>Attention, il reste 22 champs à remplir!</v>
       </c>
     </row>
     <row r="6" spans="2:25" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -12433,24 +12437,24 @@
         <f>IF(LEN('Sprint 1 - Planification'!H13)&lt;&gt;0,'Sprint 1 - Planification'!H13,"")</f>
         <v>Sprint 1</v>
       </c>
-      <c r="E14" s="73" t="str">
+      <c r="E14" s="73">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E13),"",'Sprint 1 - Bilan'!E13)</f>
-        <v/>
-      </c>
-      <c r="F14" s="77" t="str">
+        <v>2.0833333333333301E-2</v>
+      </c>
+      <c r="F14" s="77">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!F13),"",'Sprint 1 - Bilan'!F13)</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G14" s="112"/>
       <c r="H14" s="113"/>
       <c r="I14" s="114"/>
       <c r="M14" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N14" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O14" s="3" t="b">
         <f t="shared" si="2"/>
@@ -12458,7 +12462,7 @@
       </c>
       <c r="P14" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R14" s="8"/>
       <c r="U14" s="4" t="s">
@@ -12566,11 +12570,11 @@
       <c r="R16" s="8"/>
       <c r="V16" s="4">
         <f>P44</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="W16" s="4" t="str">
         <f>IF(V16=0,"",IF(V16=1,"Une tâche est en retard!",CONCATENATE(V16," tâches sont en retard!")))</f>
-        <v>12 tâches sont en retard!</v>
+        <v>11 tâches sont en retard!</v>
       </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.2">
@@ -13711,11 +13715,11 @@
     <row r="44" spans="2:18" x14ac:dyDescent="0.2">
       <c r="M44" s="3">
         <f>COUNTIF(M9:M43,TRUE)</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="N44" s="3">
         <f t="shared" ref="N44:O44" si="5">COUNTIF(N9:N43,TRUE)</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O44" s="3">
         <f t="shared" si="5"/>
@@ -13723,21 +13727,21 @@
       </c>
       <c r="P44" s="3">
         <f>COUNTIF(P9:P43,FALSE)</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="R44" s="8"/>
     </row>
     <row r="45" spans="2:18" x14ac:dyDescent="0.2">
       <c r="M45" s="3">
         <f>SUM(M44:O44)</f>
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="R45" s="8"/>
     </row>
     <row r="46" spans="2:18" x14ac:dyDescent="0.2">
       <c r="M46" s="3" t="str">
         <f>IF(M45=0, "aucun champ", IF(M45=1, "1 champ", M45 &amp; " champs"))</f>
-        <v>24 champs</v>
+        <v>22 champs</v>
       </c>
       <c r="R46" s="8"/>
     </row>
@@ -13981,7 +13985,7 @@
       <c r="H5" s="35"/>
       <c r="I5" s="64" t="str">
         <f>IF(M45=0,CONCATENATE("Ce sprint totalise ", W15, " de travail réalisé. ",W16),CONCATENATE("Attention, il reste ",M46," à remplir!"))</f>
-        <v>Attention, il reste 36 champs à remplir!</v>
+        <v>Attention, il reste 34 champs à remplir!</v>
       </c>
     </row>
     <row r="6" spans="2:25" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -14306,24 +14310,24 @@
         <f>IF(LEN('Sprint 1 - Planification'!H13)&lt;&gt;0,'Sprint 1 - Planification'!H13,"")</f>
         <v>Sprint 1</v>
       </c>
-      <c r="E14" s="73" t="str">
+      <c r="E14" s="73">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E14)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G14)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E14)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G14))</f>
-        <v/>
-      </c>
-      <c r="F14" s="77" t="str">
+        <v>2.0833333333333301E-2</v>
+      </c>
+      <c r="F14" s="77">
         <f>IF(LEN('Sprint 2 - Bilan'!$H14)&lt;&gt;0,'Sprint 2 - Bilan'!$H14,IF(LEN('Sprint 2 - Bilan'!$F14)=0,"",'Sprint 2 - Bilan'!$F14))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G14" s="112"/>
       <c r="H14" s="113"/>
       <c r="I14" s="114"/>
       <c r="M14" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N14" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O14" s="3" t="b">
         <f t="shared" si="2"/>
@@ -14331,7 +14335,7 @@
       </c>
       <c r="P14" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R14" s="8"/>
       <c r="U14" s="4" t="s">
@@ -14439,11 +14443,11 @@
       <c r="R16" s="8"/>
       <c r="V16" s="4">
         <f>P44</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="W16" s="4" t="str">
         <f>IF(V16=0,"",IF(V16=1,"Une tâche n'a pas été terminée!",CONCATENATE(V16," tâches n'ont pas été terminé!")))</f>
-        <v>18 tâches n'ont pas été terminé!</v>
+        <v>17 tâches n'ont pas été terminé!</v>
       </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.2">
@@ -15583,11 +15587,11 @@
     <row r="44" spans="2:18" x14ac:dyDescent="0.2">
       <c r="M44" s="3">
         <f>COUNTIF(M9:M43,TRUE)</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N44" s="3">
         <f t="shared" ref="N44:O44" si="5">COUNTIF(N9:N43,TRUE)</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O44" s="3">
         <f t="shared" si="5"/>
@@ -15595,21 +15599,21 @@
       </c>
       <c r="P44" s="3">
         <f>COUNTIF(P9:P43,FALSE)</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R44" s="8"/>
     </row>
     <row r="45" spans="2:18" x14ac:dyDescent="0.2">
       <c r="M45" s="3">
         <f>SUM(M44:O44)</f>
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="R45" s="8"/>
     </row>
     <row r="46" spans="2:18" x14ac:dyDescent="0.2">
       <c r="M46" s="3" t="str">
         <f>IF(M45=0, "aucun champ", IF(M45=1, "1 champ", M45 &amp; " champs"))</f>
-        <v>36 champs</v>
+        <v>34 champs</v>
       </c>
       <c r="R46" s="8"/>
     </row>
@@ -15935,7 +15939,7 @@
       </c>
       <c r="C10" s="95" t="str">
         <f t="shared" si="0"/>
-        <v>15h00</v>
+        <v>15h30</v>
       </c>
       <c r="D10" s="96" t="str">
         <f t="shared" si="0"/>
@@ -15947,13 +15951,13 @@
       </c>
       <c r="F10" s="101" t="str">
         <f t="shared" si="0"/>
-        <v>15h00</v>
+        <v>15h30</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="L10" s="1">
         <f>'Sprint 1 - Bilan'!T8</f>
-        <v>0.62499999999999922</v>
+        <v>0.64583333333333248</v>
       </c>
       <c r="M10" s="1">
         <f>'Sprint 2 - Bilan'!V9</f>
@@ -15965,14 +15969,14 @@
       </c>
       <c r="O10" s="1">
         <f>SUM(L10:N10)</f>
-        <v>0.62499999999999922</v>
+        <v>0.64583333333333248</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>66</v>
       </c>
       <c r="Q10" s="1">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>15.5</v>
       </c>
       <c r="R10" s="1">
         <f t="shared" si="1"/>
@@ -16003,37 +16007,37 @@
       </c>
       <c r="C11" s="104">
         <f>L11</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D11" s="105">
         <f>M11</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E11" s="106">
         <f>N11</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F11" s="107">
         <f>O11</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="L11" s="1">
         <f>'Sprint 1 - Bilan'!T15</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M11" s="1">
         <f>'Sprint 2 - Bilan'!V16</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="N11" s="1">
         <f>'Sprint 3 - Bilan'!V16</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O11" s="1">
         <f>N11</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>

</xml_diff>

<commit_message>
creation du kernel pour le blur
</commit_message>
<xml_diff>
--- a/B65_S1_Conception_Afsaneh_Sheikhmiri/B65_S1_Planification_AfsanehSheikhmiri.xlsx
+++ b/B65_S1_Conception_Afsaneh_Sheikhmiri/B65_S1_Planification_AfsanehSheikhmiri.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" tabRatio="494"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" tabRatio="494" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1 - Planification" sheetId="1" r:id="rId1"/>
@@ -3491,6 +3491,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3605,8 +3606,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="1835328800"/>
-        <c:axId val="1835330848"/>
+        <c:axId val="-596597744"/>
+        <c:axId val="-596595696"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -3656,13 +3657,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>6.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>11.0</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.0</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3679,11 +3680,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1835328800"/>
-        <c:axId val="1835330848"/>
+        <c:axId val="-596597744"/>
+        <c:axId val="-596595696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1835328800"/>
+        <c:axId val="-596597744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3726,7 +3727,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1835330848"/>
+        <c:crossAx val="-596595696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3734,7 +3735,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1835330848"/>
+        <c:axId val="-596595696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3785,7 +3786,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1835328800"/>
+        <c:crossAx val="-596597744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3799,6 +3800,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3905,6 +3907,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4065,10 +4068,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>15.5</c:v>
+                  <c:v>21.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.0</c:v>
@@ -4087,11 +4090,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-15"/>
-        <c:axId val="1833418544"/>
-        <c:axId val="1833421296"/>
+        <c:axId val="-599305328"/>
+        <c:axId val="-599246944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1833418544"/>
+        <c:axId val="-599305328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4134,7 +4137,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1833421296"/>
+        <c:crossAx val="-599246944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4142,7 +4145,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1833421296"/>
+        <c:axId val="-599246944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4193,7 +4196,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1833418544"/>
+        <c:crossAx val="-599305328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4207,6 +4210,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4313,6 +4317,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4610,6 +4615,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4716,6 +4722,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5037,6 +5044,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7759,7 +7767,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AJ90"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
@@ -10611,7 +10619,7 @@
   <dimension ref="B1:W56"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10668,7 +10676,7 @@
       <c r="F5" s="35"/>
       <c r="G5" s="64" t="str">
         <f>IF(K44=0,CONCATENATE("Ce sprint totalise ", U14, " de travail réalisé. ",U15),CONCATENATE("Attention, il reste ",K45," à remplir!"))</f>
-        <v>Attention, il reste 8 champs à remplir!</v>
+        <v>Attention, il reste 2 champs à remplir!</v>
       </c>
     </row>
     <row r="6" spans="2:23" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -10732,15 +10740,15 @@
       </c>
       <c r="Q8" s="61">
         <f t="array" ref="Q8">SUM(($D$8:$D$42=$P8)*$E$8:$E$42)</f>
-        <v>0.64583333333333248</v>
+        <v>0.88541666666666596</v>
       </c>
       <c r="R8" s="62">
         <f>Q8*24*60</f>
-        <v>929.99999999999875</v>
+        <v>1274.9999999999989</v>
       </c>
       <c r="T8" s="9">
         <f>SUM(E8:E42)</f>
-        <v>0.64583333333333248</v>
+        <v>0.88541666666666596</v>
       </c>
     </row>
     <row r="9" spans="2:23" x14ac:dyDescent="0.2">
@@ -10788,7 +10796,7 @@
       </c>
       <c r="T9" s="10">
         <f>T8</f>
-        <v>0.64583333333333248</v>
+        <v>0.88541666666666596</v>
       </c>
     </row>
     <row r="10" spans="2:23" x14ac:dyDescent="0.2">
@@ -10838,7 +10846,7 @@
       </c>
       <c r="T10" s="63">
         <f>DAY(T8)*24+HOUR(T8)</f>
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="2:23" x14ac:dyDescent="0.2">
@@ -10880,7 +10888,7 @@
       <c r="P11" s="8"/>
       <c r="T11" s="4">
         <f>MINUTE(T8)</f>
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="2:23" x14ac:dyDescent="0.2">
@@ -10897,7 +10905,7 @@
         <v>Sprint 1</v>
       </c>
       <c r="E12" s="118">
-        <v>2.0833333333333301E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="F12" s="116">
         <v>1</v>
@@ -10921,11 +10929,11 @@
       </c>
       <c r="T12" s="63">
         <f>T10</f>
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="U12" s="4" t="str">
         <f>T12 &amp; " " &amp; S12 &amp; IF(T12 &gt; 1, "s", "")</f>
-        <v>15 heures</v>
+        <v>21 heures</v>
       </c>
     </row>
     <row r="13" spans="2:23" x14ac:dyDescent="0.2">
@@ -10942,7 +10950,7 @@
         <v>Sprint 1</v>
       </c>
       <c r="E13" s="112">
-        <v>2.0833333333333301E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="F13" s="113">
         <v>1</v>
@@ -10966,11 +10974,11 @@
       </c>
       <c r="T13" s="4">
         <f>T11</f>
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="U13" s="4" t="str">
         <f>T13 &amp; " " &amp; S13 &amp; IF(T13 &gt; 1, "s", "")</f>
-        <v>30 minutes</v>
+        <v>15 minutes</v>
       </c>
     </row>
     <row r="14" spans="2:23" x14ac:dyDescent="0.2">
@@ -10986,16 +10994,20 @@
         <f>IF(LEN('Sprint 1 - Planification'!H14)&lt;&gt;0,'Sprint 1 - Planification'!H14,"")</f>
         <v>Sprint 1</v>
       </c>
-      <c r="E14" s="118"/>
-      <c r="F14" s="116"/>
+      <c r="E14" s="118">
+        <v>8.3333333333333301E-2</v>
+      </c>
+      <c r="F14" s="116">
+        <v>1</v>
+      </c>
       <c r="G14" s="117"/>
       <c r="K14" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L14" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M14" s="3" t="b">
         <f t="shared" si="2"/>
@@ -11004,11 +11016,11 @@
       <c r="P14" s="8"/>
       <c r="U14" s="4" t="str">
         <f>IF(T12&gt;0,IF(T13&gt;0,U12&amp;" et "&amp;U13,U12),U13)</f>
-        <v>15 heures et 30 minutes</v>
+        <v>21 heures et 15 minutes</v>
       </c>
       <c r="W14" s="4" t="str">
         <f>T12&amp;"h"&amp;TEXT(T13,"00")</f>
-        <v>15h30</v>
+        <v>21h15</v>
       </c>
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.2">
@@ -11024,16 +11036,20 @@
         <f>IF(LEN('Sprint 1 - Planification'!H15)&lt;&gt;0,'Sprint 1 - Planification'!H15,"")</f>
         <v>Sprint 1</v>
       </c>
-      <c r="E15" s="112"/>
-      <c r="F15" s="113"/>
+      <c r="E15" s="112">
+        <v>4.1666666666666699E-2</v>
+      </c>
+      <c r="F15" s="113">
+        <v>1</v>
+      </c>
       <c r="G15" s="114"/>
       <c r="K15" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L15" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M15" s="3" t="b">
         <f t="shared" si="2"/>
@@ -11042,11 +11058,11 @@
       <c r="P15" s="8"/>
       <c r="T15" s="4">
         <f t="array" ref="T15">SUM(($D$8:$D$42="Sprint 1")*($F$8:$F$42&lt;1))</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="U15" s="4" t="str">
         <f>IF(T15=0,"",IF(T15=1,"Une tâche est en retard!",CONCATENATE(T15," tâches sont en retard!")))</f>
-        <v>6 tâches sont en retard!</v>
+        <v>3 tâches sont en retard!</v>
       </c>
     </row>
     <row r="16" spans="2:23" x14ac:dyDescent="0.2">
@@ -11062,16 +11078,20 @@
         <f>IF(LEN('Sprint 1 - Planification'!H16)&lt;&gt;0,'Sprint 1 - Planification'!H16,"")</f>
         <v>Sprint 1</v>
       </c>
-      <c r="E16" s="115"/>
-      <c r="F16" s="116"/>
+      <c r="E16" s="115">
+        <v>3.125E-2</v>
+      </c>
+      <c r="F16" s="116">
+        <v>1</v>
+      </c>
       <c r="G16" s="117"/>
       <c r="K16" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L16" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M16" s="3" t="b">
         <f t="shared" si="2"/>
@@ -11862,11 +11882,11 @@
     <row r="43" spans="2:16" x14ac:dyDescent="0.2">
       <c r="K43" s="3">
         <f>COUNTIF(K8:K42,TRUE)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L43" s="3">
         <f t="shared" ref="L43:M43" si="4">COUNTIF(L8:L42,TRUE)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M43" s="3">
         <f t="shared" si="4"/>
@@ -11877,14 +11897,14 @@
     <row r="44" spans="2:16" x14ac:dyDescent="0.2">
       <c r="K44" s="3">
         <f>SUM(K43:M43)</f>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="P44" s="8"/>
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.2">
       <c r="K45" s="3" t="str">
         <f>IF(K44=0, "aucun champ", IF(K44=1, "1 champ", K44 &amp; " champs"))</f>
-        <v>8 champs</v>
+        <v>2 champs</v>
       </c>
       <c r="P45" s="8"/>
     </row>
@@ -12047,7 +12067,7 @@
   <dimension ref="B1:Z57"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12112,7 +12132,7 @@
       <c r="H5" s="35"/>
       <c r="I5" s="64" t="str">
         <f>IF(M45=0,CONCATENATE("Ce sprint totalise ", W15, " de travail réalisé. ",W16),CONCATENATE("Attention, il reste ",M46," à remplir!"))</f>
-        <v>Attention, il reste 22 champs à remplir!</v>
+        <v>Attention, il reste 12 champs à remplir!</v>
       </c>
     </row>
     <row r="6" spans="2:25" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -12201,15 +12221,15 @@
       </c>
       <c r="S9" s="61">
         <f t="array" ref="S9">SUM(($D$9:$D$43=$R9)*$G$9:$G$43)</f>
-        <v>0</v>
+        <v>0.16666666666666669</v>
       </c>
       <c r="T9" s="62">
         <f>S9*24*60</f>
-        <v>0</v>
+        <v>240</v>
       </c>
       <c r="V9" s="9">
         <f>SUM(G9:G43)</f>
-        <v>0</v>
+        <v>0.16666666666666669</v>
       </c>
     </row>
     <row r="10" spans="2:25" x14ac:dyDescent="0.2">
@@ -12265,7 +12285,7 @@
       </c>
       <c r="V10" s="10">
         <f>V9</f>
-        <v>0</v>
+        <v>0.16666666666666669</v>
       </c>
     </row>
     <row r="11" spans="2:25" x14ac:dyDescent="0.2">
@@ -12289,16 +12309,20 @@
         <f>IF(ISBLANK('Sprint 1 - Bilan'!F10),"",'Sprint 1 - Bilan'!F10)</f>
         <v>0.85</v>
       </c>
-      <c r="G11" s="115"/>
-      <c r="H11" s="116"/>
+      <c r="G11" s="115">
+        <v>0.125</v>
+      </c>
+      <c r="H11" s="116">
+        <v>1</v>
+      </c>
       <c r="I11" s="117"/>
       <c r="M11" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N11" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O11" s="3" t="b">
         <f t="shared" si="2"/>
@@ -12306,7 +12330,7 @@
       </c>
       <c r="P11" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R11" s="4" t="s">
         <v>3</v>
@@ -12321,7 +12345,7 @@
       </c>
       <c r="V11" s="63">
         <f>DAY(V9)*24+HOUR(V9)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="2:25" x14ac:dyDescent="0.2">
@@ -12345,16 +12369,20 @@
         <f>IF(ISBLANK('Sprint 1 - Bilan'!F11),"",'Sprint 1 - Bilan'!F11)</f>
         <v>0.8</v>
       </c>
-      <c r="G12" s="112"/>
-      <c r="H12" s="113"/>
+      <c r="G12" s="112">
+        <v>4.1666666666666699E-2</v>
+      </c>
+      <c r="H12" s="113">
+        <v>1</v>
+      </c>
       <c r="I12" s="114"/>
       <c r="M12" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N12" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O12" s="3" t="b">
         <f t="shared" si="2"/>
@@ -12362,7 +12390,7 @@
       </c>
       <c r="P12" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q12" s="8"/>
       <c r="R12" s="8"/>
@@ -12386,7 +12414,7 @@
       </c>
       <c r="E13" s="75">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E12),"",'Sprint 1 - Bilan'!E12)</f>
-        <v>2.0833333333333301E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="F13" s="79">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!F12),"",'Sprint 1 - Bilan'!F12)</f>
@@ -12417,11 +12445,11 @@
       </c>
       <c r="V13" s="63">
         <f>V11</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="W13" s="4" t="str">
         <f>V13 &amp; " " &amp; U13 &amp; IF(V13 &gt; 1, "s", "")</f>
-        <v>0 heure</v>
+        <v>4 heures</v>
       </c>
     </row>
     <row r="14" spans="2:25" x14ac:dyDescent="0.2">
@@ -12439,7 +12467,7 @@
       </c>
       <c r="E14" s="73">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E13),"",'Sprint 1 - Bilan'!E13)</f>
-        <v>2.0833333333333301E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="F14" s="77">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!F13),"",'Sprint 1 - Bilan'!F13)</f>
@@ -12490,24 +12518,24 @@
         <f>IF(LEN('Sprint 1 - Planification'!H14)&lt;&gt;0,'Sprint 1 - Planification'!H14,"")</f>
         <v>Sprint 1</v>
       </c>
-      <c r="E15" s="75" t="str">
+      <c r="E15" s="75">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E14),"",'Sprint 1 - Bilan'!E14)</f>
-        <v/>
-      </c>
-      <c r="F15" s="79" t="str">
+        <v>8.3333333333333301E-2</v>
+      </c>
+      <c r="F15" s="79">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!F14),"",'Sprint 1 - Bilan'!F14)</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G15" s="118"/>
       <c r="H15" s="116"/>
       <c r="I15" s="117"/>
       <c r="M15" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N15" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O15" s="3" t="b">
         <f t="shared" si="2"/>
@@ -12515,16 +12543,16 @@
       </c>
       <c r="P15" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R15" s="8"/>
       <c r="W15" s="4" t="str">
         <f>IF(V13&gt;0,IF(V14&gt;0,W13&amp;" et "&amp;W14,W13),W14)</f>
-        <v>0 minute</v>
+        <v>4 heures</v>
       </c>
       <c r="Y15" s="4" t="str">
         <f>V13&amp;"h"&amp;TEXT(V14,"00")</f>
-        <v>0h00</v>
+        <v>4h00</v>
       </c>
     </row>
     <row r="16" spans="2:25" x14ac:dyDescent="0.2">
@@ -12540,24 +12568,24 @@
         <f>IF(LEN('Sprint 1 - Planification'!H15)&lt;&gt;0,'Sprint 1 - Planification'!H15,"")</f>
         <v>Sprint 1</v>
       </c>
-      <c r="E16" s="73" t="str">
+      <c r="E16" s="73">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E15),"",'Sprint 1 - Bilan'!E15)</f>
-        <v/>
-      </c>
-      <c r="F16" s="77" t="str">
+        <v>4.1666666666666699E-2</v>
+      </c>
+      <c r="F16" s="77">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!F15),"",'Sprint 1 - Bilan'!F15)</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G16" s="112"/>
       <c r="H16" s="113"/>
       <c r="I16" s="114"/>
       <c r="M16" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N16" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O16" s="3" t="b">
         <f t="shared" si="2"/>
@@ -12565,16 +12593,16 @@
       </c>
       <c r="P16" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R16" s="8"/>
       <c r="V16" s="4">
         <f>P44</f>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="W16" s="4" t="str">
         <f>IF(V16=0,"",IF(V16=1,"Une tâche est en retard!",CONCATENATE(V16," tâches sont en retard!")))</f>
-        <v>11 tâches sont en retard!</v>
+        <v>6 tâches sont en retard!</v>
       </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.2">
@@ -12590,24 +12618,24 @@
         <f>IF(LEN('Sprint 1 - Planification'!H16)&lt;&gt;0,'Sprint 1 - Planification'!H16,"")</f>
         <v>Sprint 1</v>
       </c>
-      <c r="E17" s="74" t="str">
+      <c r="E17" s="74">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E16),"",'Sprint 1 - Bilan'!E16)</f>
-        <v/>
-      </c>
-      <c r="F17" s="78" t="str">
+        <v>3.125E-2</v>
+      </c>
+      <c r="F17" s="78">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!F16),"",'Sprint 1 - Bilan'!F16)</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G17" s="115"/>
       <c r="H17" s="116"/>
       <c r="I17" s="117"/>
       <c r="M17" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N17" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O17" s="3" t="b">
         <f t="shared" si="2"/>
@@ -12615,7 +12643,7 @@
       </c>
       <c r="P17" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R17" s="8"/>
     </row>
@@ -13715,11 +13743,11 @@
     <row r="44" spans="2:18" x14ac:dyDescent="0.2">
       <c r="M44" s="3">
         <f>COUNTIF(M9:M43,TRUE)</f>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="N44" s="3">
         <f t="shared" ref="N44:O44" si="5">COUNTIF(N9:N43,TRUE)</f>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="O44" s="3">
         <f t="shared" si="5"/>
@@ -13727,21 +13755,21 @@
       </c>
       <c r="P44" s="3">
         <f>COUNTIF(P9:P43,FALSE)</f>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="R44" s="8"/>
     </row>
     <row r="45" spans="2:18" x14ac:dyDescent="0.2">
       <c r="M45" s="3">
         <f>SUM(M44:O44)</f>
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="R45" s="8"/>
     </row>
     <row r="46" spans="2:18" x14ac:dyDescent="0.2">
       <c r="M46" s="3" t="str">
         <f>IF(M45=0, "aucun champ", IF(M45=1, "1 champ", M45 &amp; " champs"))</f>
-        <v>22 champs</v>
+        <v>12 champs</v>
       </c>
       <c r="R46" s="8"/>
     </row>
@@ -13985,7 +14013,7 @@
       <c r="H5" s="35"/>
       <c r="I5" s="64" t="str">
         <f>IF(M45=0,CONCATENATE("Ce sprint totalise ", W15, " de travail réalisé. ",W16),CONCATENATE("Attention, il reste ",M46," à remplir!"))</f>
-        <v>Attention, il reste 34 champs à remplir!</v>
+        <v>Attention, il reste 24 champs à remplir!</v>
       </c>
     </row>
     <row r="6" spans="2:25" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -14156,22 +14184,22 @@
       </c>
       <c r="E11" s="74">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E11)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G11)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E11)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G11))</f>
-        <v>0.33333333333333298</v>
+        <v>0.45833333333333298</v>
       </c>
       <c r="F11" s="78">
         <f>IF(LEN('Sprint 2 - Bilan'!$H11)&lt;&gt;0,'Sprint 2 - Bilan'!$H11,IF(LEN('Sprint 2 - Bilan'!$F11)=0,"",'Sprint 2 - Bilan'!$F11))</f>
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="G11" s="115"/>
       <c r="H11" s="116"/>
       <c r="I11" s="117"/>
       <c r="M11" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N11" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O11" s="3" t="b">
         <f t="shared" si="2"/>
@@ -14179,7 +14207,7 @@
       </c>
       <c r="P11" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R11" s="4" t="s">
         <v>3</v>
@@ -14212,22 +14240,22 @@
       </c>
       <c r="E12" s="73">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E12)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G12)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E12)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G12))</f>
-        <v>8.3333333333333301E-2</v>
+        <v>0.125</v>
       </c>
       <c r="F12" s="77">
         <f>IF(LEN('Sprint 2 - Bilan'!$H12)&lt;&gt;0,'Sprint 2 - Bilan'!$H12,IF(LEN('Sprint 2 - Bilan'!$F12)=0,"",'Sprint 2 - Bilan'!$F12))</f>
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="G12" s="112"/>
       <c r="H12" s="113"/>
       <c r="I12" s="114"/>
       <c r="M12" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N12" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O12" s="3" t="b">
         <f t="shared" si="2"/>
@@ -14235,7 +14263,7 @@
       </c>
       <c r="P12" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q12" s="8"/>
       <c r="R12" s="8"/>
@@ -14259,7 +14287,7 @@
       </c>
       <c r="E13" s="75">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E13)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G13)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E13)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G13))</f>
-        <v>2.0833333333333301E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="F13" s="79">
         <f>IF(LEN('Sprint 2 - Bilan'!$H13)&lt;&gt;0,'Sprint 2 - Bilan'!$H13,IF(LEN('Sprint 2 - Bilan'!$F13)=0,"",'Sprint 2 - Bilan'!$F13))</f>
@@ -14312,7 +14340,7 @@
       </c>
       <c r="E14" s="73">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E14)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G14)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E14)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G14))</f>
-        <v>2.0833333333333301E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="F14" s="77">
         <f>IF(LEN('Sprint 2 - Bilan'!$H14)&lt;&gt;0,'Sprint 2 - Bilan'!$H14,IF(LEN('Sprint 2 - Bilan'!$F14)=0,"",'Sprint 2 - Bilan'!$F14))</f>
@@ -14363,24 +14391,24 @@
         <f>IF(LEN('Sprint 1 - Planification'!H14)&lt;&gt;0,'Sprint 1 - Planification'!H14,"")</f>
         <v>Sprint 1</v>
       </c>
-      <c r="E15" s="75" t="str">
+      <c r="E15" s="75">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E15)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G15)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E15)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G15))</f>
-        <v/>
-      </c>
-      <c r="F15" s="79" t="str">
+        <v>8.3333333333333301E-2</v>
+      </c>
+      <c r="F15" s="79">
         <f>IF(LEN('Sprint 2 - Bilan'!$H15)&lt;&gt;0,'Sprint 2 - Bilan'!$H15,IF(LEN('Sprint 2 - Bilan'!$F15)=0,"",'Sprint 2 - Bilan'!$F15))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G15" s="118"/>
       <c r="H15" s="116"/>
       <c r="I15" s="117"/>
       <c r="M15" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N15" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O15" s="3" t="b">
         <f t="shared" si="2"/>
@@ -14388,7 +14416,7 @@
       </c>
       <c r="P15" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R15" s="8"/>
       <c r="W15" s="4" t="str">
@@ -14413,24 +14441,24 @@
         <f>IF(LEN('Sprint 1 - Planification'!H15)&lt;&gt;0,'Sprint 1 - Planification'!H15,"")</f>
         <v>Sprint 1</v>
       </c>
-      <c r="E16" s="73" t="str">
+      <c r="E16" s="73">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E16)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G16)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E16)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G16))</f>
-        <v/>
-      </c>
-      <c r="F16" s="77" t="str">
+        <v>4.1666666666666699E-2</v>
+      </c>
+      <c r="F16" s="77">
         <f>IF(LEN('Sprint 2 - Bilan'!$H16)&lt;&gt;0,'Sprint 2 - Bilan'!$H16,IF(LEN('Sprint 2 - Bilan'!$F16)=0,"",'Sprint 2 - Bilan'!$F16))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G16" s="112"/>
       <c r="H16" s="113"/>
       <c r="I16" s="114"/>
       <c r="M16" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N16" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O16" s="3" t="b">
         <f t="shared" si="2"/>
@@ -14438,16 +14466,16 @@
       </c>
       <c r="P16" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R16" s="8"/>
       <c r="V16" s="4">
         <f>P44</f>
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="W16" s="4" t="str">
         <f>IF(V16=0,"",IF(V16=1,"Une tâche n'a pas été terminée!",CONCATENATE(V16," tâches n'ont pas été terminé!")))</f>
-        <v>17 tâches n'ont pas été terminé!</v>
+        <v>12 tâches n'ont pas été terminé!</v>
       </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.2">
@@ -14463,24 +14491,24 @@
         <f>IF(LEN('Sprint 1 - Planification'!H16)&lt;&gt;0,'Sprint 1 - Planification'!H16,"")</f>
         <v>Sprint 1</v>
       </c>
-      <c r="E17" s="74" t="str">
+      <c r="E17" s="74">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E17)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G17)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E17)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G17))</f>
-        <v/>
-      </c>
-      <c r="F17" s="78" t="str">
+        <v>3.125E-2</v>
+      </c>
+      <c r="F17" s="78">
         <f>IF(LEN('Sprint 2 - Bilan'!$H17)&lt;&gt;0,'Sprint 2 - Bilan'!$H17,IF(LEN('Sprint 2 - Bilan'!$F17)=0,"",'Sprint 2 - Bilan'!$F17))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G17" s="115"/>
       <c r="H17" s="116"/>
       <c r="I17" s="117"/>
       <c r="M17" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N17" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O17" s="3" t="b">
         <f t="shared" si="2"/>
@@ -14488,7 +14516,7 @@
       </c>
       <c r="P17" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R17" s="8"/>
     </row>
@@ -15587,11 +15615,11 @@
     <row r="44" spans="2:18" x14ac:dyDescent="0.2">
       <c r="M44" s="3">
         <f>COUNTIF(M9:M43,TRUE)</f>
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="N44" s="3">
         <f t="shared" ref="N44:O44" si="5">COUNTIF(N9:N43,TRUE)</f>
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="O44" s="3">
         <f t="shared" si="5"/>
@@ -15599,21 +15627,21 @@
       </c>
       <c r="P44" s="3">
         <f>COUNTIF(P9:P43,FALSE)</f>
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="R44" s="8"/>
     </row>
     <row r="45" spans="2:18" x14ac:dyDescent="0.2">
       <c r="M45" s="3">
         <f>SUM(M44:O44)</f>
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="R45" s="8"/>
     </row>
     <row r="46" spans="2:18" x14ac:dyDescent="0.2">
       <c r="M46" s="3" t="str">
         <f>IF(M45=0, "aucun champ", IF(M45=1, "1 champ", M45 &amp; " champs"))</f>
-        <v>34 champs</v>
+        <v>24 champs</v>
       </c>
       <c r="R46" s="8"/>
     </row>
@@ -15736,7 +15764,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Y23"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="A3" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="AY27" sqref="AY27"/>
     </sheetView>
   </sheetViews>
@@ -15939,11 +15967,11 @@
       </c>
       <c r="C10" s="95" t="str">
         <f t="shared" si="0"/>
-        <v>15h30</v>
+        <v>21h15</v>
       </c>
       <c r="D10" s="96" t="str">
         <f t="shared" si="0"/>
-        <v>0h00</v>
+        <v>4h00</v>
       </c>
       <c r="E10" s="97" t="str">
         <f t="shared" si="0"/>
@@ -15951,17 +15979,17 @@
       </c>
       <c r="F10" s="101" t="str">
         <f t="shared" si="0"/>
-        <v>15h30</v>
+        <v>25h15</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="L10" s="1">
         <f>'Sprint 1 - Bilan'!T8</f>
-        <v>0.64583333333333248</v>
+        <v>0.88541666666666596</v>
       </c>
       <c r="M10" s="1">
         <f>'Sprint 2 - Bilan'!V9</f>
-        <v>0</v>
+        <v>0.16666666666666669</v>
       </c>
       <c r="N10" s="1">
         <f>'Sprint 3 - Bilan'!V9</f>
@@ -15969,18 +15997,18 @@
       </c>
       <c r="O10" s="1">
         <f>SUM(L10:N10)</f>
-        <v>0.64583333333333248</v>
+        <v>1.0520833333333326</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>66</v>
       </c>
       <c r="Q10" s="1">
         <f t="shared" si="1"/>
-        <v>15.5</v>
+        <v>21.25</v>
       </c>
       <c r="R10" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S10" s="1">
         <f t="shared" si="1"/>
@@ -16007,37 +16035,37 @@
       </c>
       <c r="C11" s="104">
         <f>L11</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D11" s="105">
         <f>M11</f>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E11" s="106">
         <f>N11</f>
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F11" s="107">
         <f>O11</f>
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="L11" s="1">
         <f>'Sprint 1 - Bilan'!T15</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M11" s="1">
         <f>'Sprint 2 - Bilan'!V16</f>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="N11" s="1">
         <f>'Sprint 3 - Bilan'!V16</f>
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="O11" s="1">
         <f>N11</f>
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
@@ -16183,7 +16211,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H36"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="A17" workbookViewId="0">
       <selection activeCell="AQ41" sqref="AQ41"/>
     </sheetView>
   </sheetViews>

</xml_diff>